<commit_message>
added more alt coins, analysis - tbd, analysis on Polygon
</commit_message>
<xml_diff>
--- a/Cryptos.xlsx
+++ b/Cryptos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinu\Projects\Personal\my-stock-market-learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinu\Projects\Personal\my-crypto-trading-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC89C159-6E00-433E-B59F-E144C84C48F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BC9FD7-3B22-419C-B2DF-363C830CB877}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{76CA333A-EB30-4400-846A-F17C9D947678}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="206">
   <si>
     <t>Rank</t>
   </si>
@@ -602,6 +602,57 @@
   </si>
   <si>
     <t>SOL is another good one to hold..Also try to accumalate NFTs as binance launching their marketplace ..one project which again might list on binance and cab be huge in june is Refinable (FINE)</t>
+  </si>
+  <si>
+    <t>Coti</t>
+  </si>
+  <si>
+    <t>COTI</t>
+  </si>
+  <si>
+    <t>Wilder World</t>
+  </si>
+  <si>
+    <t>WILD</t>
+  </si>
+  <si>
+    <t>MXX</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Decred</t>
+  </si>
+  <si>
+    <t>DCR</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>EGCC</t>
+  </si>
+  <si>
+    <t>ORN</t>
+  </si>
+  <si>
+    <t>Chia</t>
+  </si>
+  <si>
+    <t>Akash Network</t>
+  </si>
+  <si>
+    <t>Cosmos</t>
+  </si>
+  <si>
+    <t>Avalanche</t>
+  </si>
+  <si>
+    <t>Comepitors for Polygon</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A33B2C3-C180-4C16-844D-2B6F8854DF67}">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1198,6 +1249,9 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
+      <c r="E6" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
@@ -1654,6 +1708,85 @@
       </c>
       <c r="L59" s="5" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C60" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C61" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C62" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C64" t="s">
+        <v>197</v>
+      </c>
+      <c r="D64" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C65" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C66" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C69" t="s">
+        <v>203</v>
+      </c>
+      <c r="E69" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C70" t="s">
+        <v>204</v>
+      </c>
+      <c r="E70" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1668,7 +1801,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C24" sqref="C24:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
notes on liquidity pools, crypto attacks
</commit_message>
<xml_diff>
--- a/Cryptos.xlsx
+++ b/Cryptos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vinu\Projects\Personal\my-crypto-trading-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BC9FD7-3B22-419C-B2DF-363C830CB877}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D59B45A-BE58-4CC9-B001-21ACA835DF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{76CA333A-EB30-4400-846A-F17C9D947678}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Memes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="213">
   <si>
     <t>Rank</t>
   </si>
@@ -653,6 +654,27 @@
   </si>
   <si>
     <t>Comepitors for Polygon</t>
+  </si>
+  <si>
+    <t>Algorand</t>
+  </si>
+  <si>
+    <t>Zilliqa</t>
+  </si>
+  <si>
+    <t>Elrond</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>Tfuel</t>
+  </si>
+  <si>
+    <t>Marlin</t>
+  </si>
+  <si>
+    <t>POND</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A33B2C3-C180-4C16-844D-2B6F8854DF67}">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1787,6 +1809,39 @@
       </c>
       <c r="E70" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C71" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C72" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C73" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C74" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C75" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C76" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>